<commit_message>
renamed data files, additional data file and figure creation script
</commit_message>
<xml_diff>
--- a/results/performance/concentration.xlsx
+++ b/results/performance/concentration.xlsx
@@ -13,208 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="134">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>01.04.2021</t>
-  </si>
-  <si>
-    <t>08.04.2021</t>
-  </si>
-  <si>
-    <t>09.04.2021</t>
-  </si>
-  <si>
-    <t>01.04.2021</t>
-  </si>
-  <si>
-    <t>08.04.2021</t>
-  </si>
-  <si>
-    <t>09.04.2021</t>
-  </si>
-  <si>
-    <t>01.04.2021</t>
-  </si>
-  <si>
-    <t>08.04.2021</t>
-  </si>
-  <si>
-    <t>09.04.2021</t>
-  </si>
-  <si>
-    <t>01.04.2021</t>
-  </si>
-  <si>
-    <t>08.04.2021</t>
-  </si>
-  <si>
-    <t>09.04.2021</t>
-  </si>
-  <si>
-    <t>01.04.2021</t>
-  </si>
-  <si>
-    <t>08.04.2021</t>
-  </si>
-  <si>
-    <t>09.04.2021</t>
-  </si>
-  <si>
-    <t>01.04.2021</t>
-  </si>
-  <si>
-    <t>08.04.2021</t>
-  </si>
-  <si>
-    <t>09.04.2021</t>
-  </si>
-  <si>
-    <t>Samples</t>
-  </si>
-  <si>
-    <t>EGFPNup107</t>
-  </si>
-  <si>
-    <t>MeasurementsFilenames</t>
-  </si>
-  <si>
-    <t>01_EGFP-Nup107-nb-Img3-1nM_LP16_PH0.85_20210401_Minflux.msr</t>
-  </si>
-  <si>
-    <t>01_EGFP-Nup107-nb-Img3-1nM_LP16_PH0.85_20210408_Minflux.msr</t>
-  </si>
-  <si>
-    <t>01_EGFP-Nup107-nb-Img3-1nM_LP16_PH0.85_20210409_Minflux.msr</t>
-  </si>
-  <si>
-    <t>02_EGFP-Nup107-nb-Img3-2nM_LP16_PH0.85_20210401_Minflux.msr</t>
-  </si>
-  <si>
-    <t>02_EGFP-Nup107-nb-Img3-2nM_LP16_PH0.85_20210408_Minflux.msr</t>
-  </si>
-  <si>
-    <t>02_EGFP-Nup107-nb-Img3-2nM_LP16_PH0.85_20210409_Minflux.msr</t>
-  </si>
-  <si>
-    <t>03_EGFP-Nup107-nb-Img3-4nM_LP16_PH0.85_20210401_Minflux.msr</t>
-  </si>
-  <si>
-    <t>03_EGFP-Nup107-nb-Img3-4nM_LP16_PH0.85_20210408_Minflux.msr</t>
-  </si>
-  <si>
-    <t>03_EGFP-Nup107-nb-Img3-4nM_LP16_PH0.85_20210409_Minflux.msr</t>
-  </si>
-  <si>
-    <t>04_EGFP-Nup107-nb-Img3-6nM_LP16_PH0.85_20210401_Minflux.msr</t>
-  </si>
-  <si>
-    <t>04_EGFP-Nup107-nb-Img3-6nM_LP16_PH0.85_20210408_Minflux.msr</t>
-  </si>
-  <si>
-    <t>04_EGFP-Nup107-nb-Img3-6nM_LP16_PH0.85_20210409_Minflux.msr</t>
-  </si>
-  <si>
-    <t>05_EGFP-Nup107-nb-Img3-8nM_LP16_PH0.85_20210401_Minflux.msr</t>
-  </si>
-  <si>
-    <t>05_EGFP-Nup107-nb-Img3-8nM_LP16_PH0.85_20210408_Minflux.msr</t>
-  </si>
-  <si>
-    <t>05_EGFP-Nup107-nb-Img3-8nM_LP16_PH0.85_20210409_Minflux.msr</t>
-  </si>
-  <si>
-    <t>06_EGFP-Nup107-nb-Img3-10nM_LP16_PH0.85_20210401_Minflux.msr</t>
-  </si>
-  <si>
-    <t>06_EGFP-Nup107-nb-Img3-10nM_LP16_PH0.85_20210408_Minflux.msr</t>
-  </si>
-  <si>
-    <t>06_EGFP-Nup107-nb-Img3-10nM_LP16_PH0.85_20210409_Minflux.msr</t>
-  </si>
-  <si>
-    <t>MinfluxLasernm</t>
-  </si>
-  <si>
-    <t>MinfluxLaserpower</t>
-  </si>
-  <si>
-    <t>MinfluxPinholesizeAU</t>
-  </si>
-  <si>
-    <t>Activation405</t>
-  </si>
-  <si>
-    <t>MinfluxSequence</t>
-  </si>
-  <si>
-    <t>seqIIF.mf</t>
-  </si>
-  <si>
-    <t>DNA_PAINT_Sequence</t>
-  </si>
-  <si>
-    <t>MP3</t>
-  </si>
-  <si>
-    <t>Dye</t>
-  </si>
-  <si>
-    <t>Atto655</t>
-  </si>
-  <si>
-    <t>Buffer</t>
-  </si>
-  <si>
-    <t>MP</t>
-  </si>
-  <si>
-    <t>ConcentrationnM</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Nanobody</t>
-  </si>
-  <si>
-    <t>ValidEventsRate</t>
-  </si>
-  <si>
-    <t>MedianFBG</t>
-  </si>
-  <si>
-    <t>MedianCFR</t>
-  </si>
-  <si>
-    <t>MedianScanTime</t>
-  </si>
-  <si>
-    <t>MedianLocTime</t>
-  </si>
-  <si>
-    <t>MedianSigmaX</t>
-  </si>
-  <si>
-    <t>MedianSigmaY</t>
-  </si>
-  <si>
-    <t>MedianSigmaZ</t>
-  </si>
-  <si>
-    <t>MedianSigmaR</t>
-  </si>
-  <si>
-    <t>FRCcombined</t>
-  </si>
-  <si>
-    <t>MeanLocPerEvent</t>
-  </si>
-  <si>
-    <t>TimeFilter</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="67">
   <si>
     <t>Date</t>
   </si>
@@ -435,7 +234,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -444,15 +243,13 @@
       <diagonal/>
     </border>
     <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,90 +291,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>113</v>
+        <v>46</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>115</v>
+        <v>48</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>117</v>
+        <v>50</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>119</v>
+        <v>52</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>120</v>
+        <v>53</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>122</v>
+        <v>55</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>123</v>
+        <v>56</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>124</v>
+        <v>57</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>125</v>
+        <v>58</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>126</v>
+        <v>59</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>127</v>
+        <v>60</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>128</v>
+        <v>61</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>129</v>
+        <v>62</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>130</v>
+        <v>63</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>131</v>
+        <v>64</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>132</v>
+        <v>65</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>133</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>68</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
       <c r="D2" s="0">
         <v>640</v>
@@ -592,22 +389,22 @@
         <v>0</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="L2" s="0">
         <v>1</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="N2" s="0">
         <v>0.16302060536682267</v>
@@ -637,7 +434,7 @@
         <v>2.3975658435651255</v>
       </c>
       <c r="W2" s="0">
-        <v>7.6335877862595423</v>
+        <v>8.097165991902834</v>
       </c>
       <c r="X2" s="0">
         <v>24.662798634812287</v>
@@ -648,13 +445,13 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>90</v>
+        <v>23</v>
       </c>
       <c r="D3" s="0">
         <v>640</v>
@@ -669,22 +466,22 @@
         <v>0</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="L3" s="0">
         <v>1</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="N3" s="0">
         <v>0.11557555127186983</v>
@@ -725,13 +522,13 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="D4" s="0">
         <v>640</v>
@@ -746,22 +543,22 @@
         <v>0</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="L4" s="0">
         <v>1</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="N4" s="0">
         <v>0.13440992984174921</v>
@@ -791,7 +588,7 @@
         <v>2.3116978955810992</v>
       </c>
       <c r="W4" s="0">
-        <v>10.928961748633879</v>
+        <v>8.5106382978723403</v>
       </c>
       <c r="X4" s="0">
         <v>24.850842020850042</v>
@@ -802,13 +599,13 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="D5" s="0">
         <v>640</v>
@@ -823,22 +620,22 @@
         <v>0</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="L5" s="0">
         <v>2</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="N5" s="0">
         <v>0.18651001178900342</v>
@@ -868,7 +665,7 @@
         <v>2.678005669980609</v>
       </c>
       <c r="W5" s="0">
-        <v>6.1349693251533735</v>
+        <v>6.7340067340067336</v>
       </c>
       <c r="X5" s="0">
         <v>22.703619909502262</v>
@@ -879,13 +676,13 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="D6" s="0">
         <v>640</v>
@@ -900,22 +697,22 @@
         <v>0</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="L6" s="0">
         <v>2</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="N6" s="0">
         <v>0.1924721614087036</v>
@@ -945,7 +742,7 @@
         <v>2.61933573334563</v>
       </c>
       <c r="W6" s="0">
-        <v>7.8740157480314954</v>
+        <v>7.7821011673151741</v>
       </c>
       <c r="X6" s="0">
         <v>27.91030303030303</v>
@@ -956,13 +753,13 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="D7" s="0">
         <v>640</v>
@@ -977,22 +774,22 @@
         <v>0</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="L7" s="0">
         <v>2</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="N7" s="0">
         <v>0.1659752633861738</v>
@@ -1022,7 +819,7 @@
         <v>2.6187272862811311</v>
       </c>
       <c r="W7" s="0">
-        <v>6.8027210884353737</v>
+        <v>7.5757575757575761</v>
       </c>
       <c r="X7" s="0">
         <v>24.805119255381037</v>
@@ -1033,13 +830,13 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
       <c r="D8" s="0">
         <v>640</v>
@@ -1054,22 +851,22 @@
         <v>0</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="L8" s="0">
         <v>4</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="N8" s="0">
         <v>0.1823178058952428</v>
@@ -1099,7 +896,7 @@
         <v>3.9317773292640226</v>
       </c>
       <c r="W8" s="0">
-        <v>8.6580086580086579</v>
+        <v>8.2987551867219906</v>
       </c>
       <c r="X8" s="0">
         <v>16.970912296165711</v>
@@ -1110,13 +907,13 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="D9" s="0">
         <v>640</v>
@@ -1131,22 +928,22 @@
         <v>0</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="L9" s="0">
         <v>4</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="N9" s="0">
         <v>0.22507343755275686</v>
@@ -1176,7 +973,7 @@
         <v>3.4834080456291847</v>
       </c>
       <c r="W9" s="0">
-        <v>6.8965517241379306</v>
+        <v>7.4074074074074066</v>
       </c>
       <c r="X9" s="0">
         <v>22.49514563106796</v>
@@ -1187,13 +984,13 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="D10" s="0">
         <v>640</v>
@@ -1208,22 +1005,22 @@
         <v>0</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="L10" s="0">
         <v>4</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="N10" s="0">
         <v>0.19624416270118575</v>
@@ -1253,7 +1050,7 @@
         <v>3.2610208584146578</v>
       </c>
       <c r="W10" s="0">
-        <v>6.5573770491803272</v>
+        <v>7.4074074074074066</v>
       </c>
       <c r="X10" s="0">
         <v>23.010496183206108</v>
@@ -1264,13 +1061,13 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>98</v>
+        <v>31</v>
       </c>
       <c r="D11" s="0">
         <v>640</v>
@@ -1285,22 +1082,22 @@
         <v>0</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="L11" s="0">
         <v>6</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="N11" s="0">
         <v>0.15959315130400956</v>
@@ -1330,7 +1127,7 @@
         <v>4.8600640935389219</v>
       </c>
       <c r="W11" s="0">
-        <v>9.2165898617511512</v>
+        <v>10.256410256410255</v>
       </c>
       <c r="X11" s="0">
         <v>13.883058470764619</v>
@@ -1341,13 +1138,13 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="D12" s="0">
         <v>640</v>
@@ -1362,22 +1159,22 @@
         <v>0</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="L12" s="0">
         <v>6</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="N12" s="0">
         <v>0.14273114119922631</v>
@@ -1407,7 +1204,7 @@
         <v>4.3030896430069987</v>
       </c>
       <c r="W12" s="0">
-        <v>8.4033613445378137</v>
+        <v>8.695652173913043</v>
       </c>
       <c r="X12" s="0">
         <v>13.961352657004831</v>
@@ -1418,13 +1215,13 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="D13" s="0">
         <v>640</v>
@@ -1439,22 +1236,22 @@
         <v>0</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="L13" s="0">
         <v>6</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="N13" s="0">
         <v>0.17666012352180782</v>
@@ -1484,7 +1281,7 @@
         <v>4.2836262697196075</v>
       </c>
       <c r="W13" s="0">
-        <v>8.4033613445378137</v>
+        <v>8.695652173913043</v>
       </c>
       <c r="X13" s="0">
         <v>16.483325504931894</v>
@@ -1495,13 +1292,13 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="D14" s="0">
         <v>640</v>
@@ -1516,22 +1313,22 @@
         <v>0</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="L14" s="0">
         <v>8</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="N14" s="0">
         <v>0.18771929824561404</v>
@@ -1561,7 +1358,7 @@
         <v>5.4174139338194935</v>
       </c>
       <c r="W14" s="0">
-        <v>9.5693779904306204</v>
+        <v>10.1010101010101</v>
       </c>
       <c r="X14" s="0">
         <v>16.291323315559865</v>
@@ -1572,13 +1369,13 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="D15" s="0">
         <v>640</v>
@@ -1593,22 +1390,22 @@
         <v>0</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="L15" s="0">
         <v>8</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="N15" s="0">
         <v>0.1457437273290543</v>
@@ -1638,7 +1435,7 @@
         <v>4.978380933339535</v>
       </c>
       <c r="W15" s="0">
-        <v>11.235955056179774</v>
+        <v>9.661835748792269</v>
       </c>
       <c r="X15" s="0">
         <v>15.509102730819246</v>
@@ -1649,13 +1446,13 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="D16" s="0">
         <v>640</v>
@@ -1670,22 +1467,22 @@
         <v>0</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="L16" s="0">
         <v>8</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="N16" s="0">
         <v>0.19870176703930761</v>
@@ -1715,7 +1512,7 @@
         <v>5.0006711022160077</v>
       </c>
       <c r="W16" s="0">
-        <v>9.1324200913241995</v>
+        <v>8.4388185654008439</v>
       </c>
       <c r="X16" s="0">
         <v>18.856750823271131</v>
@@ -1726,13 +1523,13 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>83</v>
+        <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="D17" s="0">
         <v>640</v>
@@ -1747,22 +1544,22 @@
         <v>0</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="L17" s="0">
         <v>10</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="N17" s="0">
         <v>0.29392075746119506</v>
@@ -1792,7 +1589,7 @@
         <v>5.6454900296118904</v>
       </c>
       <c r="W17" s="0">
-        <v>7.518796992481203</v>
+        <v>7.4626865671641784</v>
       </c>
       <c r="X17" s="0">
         <v>27.895601739970999</v>
@@ -1803,13 +1600,13 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="D18" s="0">
         <v>640</v>
@@ -1824,22 +1621,22 @@
         <v>0</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="L18" s="0">
         <v>10</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="N18" s="0">
         <v>0.17887766202549085</v>
@@ -1869,7 +1666,7 @@
         <v>5.3783679290997108</v>
       </c>
       <c r="W18" s="0">
-        <v>8.8105726872246688</v>
+        <v>7.8740157480314954</v>
       </c>
       <c r="X18" s="0">
         <v>19.444574780058652</v>
@@ -1880,13 +1677,13 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="D19" s="0">
         <v>640</v>
@@ -1901,22 +1698,22 @@
         <v>0</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="L19" s="0">
         <v>10</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="N19" s="0">
         <v>0.19572309882548344</v>
@@ -1946,7 +1743,7 @@
         <v>5.4827390841109445</v>
       </c>
       <c r="W19" s="0">
-        <v>10.869565217391305</v>
+        <v>9.5693779904306204</v>
       </c>
       <c r="X19" s="0">
         <v>25.097812097812099</v>

</xml_diff>